<commit_message>
completed all coding part and  api doc
</commit_message>
<xml_diff>
--- a/downloads/report.xlsx
+++ b/downloads/report.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="25" count="25">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="20" count="20">
   <x:si>
     <x:t>Name</x:t>
   </x:si>
@@ -40,9 +40,6 @@
     <x:t>MNG001</x:t>
   </x:si>
   <x:si>
-    <x:t>5fd0709530a434204c3007d5</x:t>
-  </x:si>
-  <x:si>
     <x:t>Jayashree Kulai</x:t>
   </x:si>
   <x:si>
@@ -52,9 +49,6 @@
     <x:t>MNG002</x:t>
   </x:si>
   <x:si>
-    <x:t>5fd0709530a434204c3007d5</x:t>
-  </x:si>
-  <x:si>
     <x:t>Sharal Linsha</x:t>
   </x:si>
   <x:si>
@@ -64,9 +58,6 @@
     <x:t>MNG003</x:t>
   </x:si>
   <x:si>
-    <x:t>5fd0709530a434204c3007d5</x:t>
-  </x:si>
-  <x:si>
     <x:t>Vinusha Monterio</x:t>
   </x:si>
   <x:si>
@@ -76,9 +67,6 @@
     <x:t>MNG004</x:t>
   </x:si>
   <x:si>
-    <x:t>5fd0709530a434204c3007d5</x:t>
-  </x:si>
-  <x:si>
     <x:t>Roy pashan</x:t>
   </x:si>
   <x:si>
@@ -86,9 +74,6 @@
   </x:si>
   <x:si>
     <x:t>MNG005</x:t>
-  </x:si>
-  <x:si>
-    <x:t>5fd0709530a434204c3007d5</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -478,25 +463,19 @@
       <x:c r="C2" s="0" t="s">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="D2" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
       <x:c r="E2" s="0" t="b">
         <x:v>0</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:5">
       <x:c r="A3" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="B3" s="0" t="s">
         <x:v>9</x:v>
       </x:c>
-      <x:c r="B3" s="0" t="s">
+      <x:c r="C3" s="0" t="s">
         <x:v>10</x:v>
-      </x:c>
-      <x:c r="C3" s="0" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="D3" s="0" t="s">
-        <x:v>12</x:v>
       </x:c>
       <x:c r="E3" s="0" t="b">
         <x:v>0</x:v>
@@ -504,16 +483,13 @@
     </x:row>
     <x:row r="4" spans="1:5">
       <x:c r="A4" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="B4" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="C4" s="0" t="s">
         <x:v>13</x:v>
-      </x:c>
-      <x:c r="B4" s="0" t="s">
-        <x:v>14</x:v>
-      </x:c>
-      <x:c r="C4" s="0" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="D4" s="0" t="s">
-        <x:v>16</x:v>
       </x:c>
       <x:c r="E4" s="0" t="b">
         <x:v>0</x:v>
@@ -521,16 +497,13 @@
     </x:row>
     <x:row r="5" spans="1:5">
       <x:c r="A5" s="0" t="s">
-        <x:v>17</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="B5" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="C5" s="0" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="D5" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="E5" s="0" t="b">
         <x:v>0</x:v>
@@ -538,16 +511,13 @@
     </x:row>
     <x:row r="6" spans="1:5">
       <x:c r="A6" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="B6" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="C6" s="0" t="s">
-        <x:v>23</x:v>
-      </x:c>
-      <x:c r="D6" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="E6" s="0" t="b">
         <x:v>0</x:v>

</xml_diff>

<commit_message>
clean code and updated the functionalities of upload file and creating enduser
</commit_message>
<xml_diff>
--- a/downloads/report.xlsx
+++ b/downloads/report.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="20" count="20">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="22" count="22">
   <x:si>
     <x:t>Name</x:t>
   </x:si>
@@ -22,22 +22,28 @@
     <x:t>E-mail</x:t>
   </x:si>
   <x:si>
-    <x:t>Employee_code</x:t>
-  </x:si>
-  <x:si>
     <x:t>Policy_Id</x:t>
   </x:si>
   <x:si>
     <x:t>Policy_Status</x:t>
   </x:si>
   <x:si>
+    <x:t>Winston Roy</x:t>
+  </x:si>
+  <x:si>
+    <x:t>pashanwinsty1998@gmail.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5fd320a7d28d01408a4c4e2a</x:t>
+  </x:si>
+  <x:si>
     <x:t>Vinayaka Naik</x:t>
   </x:si>
   <x:si>
     <x:t>vinayakamudrai@gmail.com</x:t>
   </x:si>
   <x:si>
-    <x:t>MNG001</x:t>
+    <x:t>5fd320a7d28d01408a4c4e2a</x:t>
   </x:si>
   <x:si>
     <x:t>Jayashree Kulai</x:t>
@@ -46,7 +52,7 @@
     <x:t>jayashree.cs16@sahyadri.edu.in</x:t>
   </x:si>
   <x:si>
-    <x:t>MNG002</x:t>
+    <x:t>5fd320a7d28d01408a4c4e2a</x:t>
   </x:si>
   <x:si>
     <x:t>Sharal Linsha</x:t>
@@ -55,7 +61,7 @@
     <x:t>sharalfonseca1810@gmail.com</x:t>
   </x:si>
   <x:si>
-    <x:t>MNG003</x:t>
+    <x:t>5fd320a7d28d01408a4c4e2a</x:t>
   </x:si>
   <x:si>
     <x:t>Vinusha Monterio</x:t>
@@ -64,7 +70,7 @@
     <x:t>vinushamonteiro2016@gmail.com</x:t>
   </x:si>
   <x:si>
-    <x:t>MNG004</x:t>
+    <x:t>5fd320a7d28d01408a4c4e2a</x:t>
   </x:si>
   <x:si>
     <x:t>Roy pashan</x:t>
@@ -73,7 +79,7 @@
     <x:t>mail2winstonroy@yahoo.com</x:t>
   </x:si>
   <x:si>
-    <x:t>MNG005</x:t>
+    <x:t>5fd320a7d28d01408a4c4e2a</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -436,7 +442,7 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="1" spans="1:5">
+    <x:row r="1" spans="1:4">
       <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -449,77 +455,88 @@
       <x:c r="D1" s="0" t="s">
         <x:v>3</x:v>
       </x:c>
-      <x:c r="E1" s="0" t="s">
+    </x:row>
+    <x:row r="2" spans="1:4">
+      <x:c r="A2" s="0" t="s">
         <x:v>4</x:v>
       </x:c>
-    </x:row>
-    <x:row r="2" spans="1:5">
-      <x:c r="A2" s="0" t="s">
+      <x:c r="B2" s="0" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="B2" s="0" t="s">
+      <x:c r="C2" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
-      <x:c r="C2" s="0" t="s">
+      <x:c r="D2" s="0" t="b">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:4">
+      <x:c r="A3" s="0" t="s">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="E2" s="0" t="b">
-        <x:v>0</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="3" spans="1:5">
-      <x:c r="A3" s="0" t="s">
+      <x:c r="B3" s="0" t="s">
         <x:v>8</x:v>
       </x:c>
-      <x:c r="B3" s="0" t="s">
+      <x:c r="C3" s="0" t="s">
         <x:v>9</x:v>
       </x:c>
-      <x:c r="C3" s="0" t="s">
+      <x:c r="D3" s="0" t="b">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:4">
+      <x:c r="A4" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="E3" s="0" t="b">
-        <x:v>0</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:5">
-      <x:c r="A4" s="0" t="s">
+      <x:c r="B4" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="B4" s="0" t="s">
+      <x:c r="C4" s="0" t="s">
         <x:v>12</x:v>
       </x:c>
-      <x:c r="C4" s="0" t="s">
+      <x:c r="D4" s="0" t="b">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:4">
+      <x:c r="A5" s="0" t="s">
         <x:v>13</x:v>
       </x:c>
-      <x:c r="E4" s="0" t="b">
-        <x:v>0</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="5" spans="1:5">
-      <x:c r="A5" s="0" t="s">
+      <x:c r="B5" s="0" t="s">
         <x:v>14</x:v>
       </x:c>
-      <x:c r="B5" s="0" t="s">
+      <x:c r="C5" s="0" t="s">
         <x:v>15</x:v>
       </x:c>
-      <x:c r="C5" s="0" t="s">
+      <x:c r="D5" s="0" t="b">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:4">
+      <x:c r="A6" s="0" t="s">
         <x:v>16</x:v>
       </x:c>
-      <x:c r="E5" s="0" t="b">
-        <x:v>0</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="6" spans="1:5">
-      <x:c r="A6" s="0" t="s">
+      <x:c r="B6" s="0" t="s">
         <x:v>17</x:v>
       </x:c>
-      <x:c r="B6" s="0" t="s">
+      <x:c r="C6" s="0" t="s">
         <x:v>18</x:v>
       </x:c>
-      <x:c r="C6" s="0" t="s">
+      <x:c r="D6" s="0" t="b">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:4">
+      <x:c r="A7" s="0" t="s">
         <x:v>19</x:v>
       </x:c>
-      <x:c r="E6" s="0" t="b">
+      <x:c r="B7" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="C7" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="D7" s="0" t="b">
         <x:v>0</x:v>
       </x:c>
     </x:row>

</xml_diff>

<commit_message>
clean code and completed the assignmnet
</commit_message>
<xml_diff>
--- a/downloads/report.xlsx
+++ b/downloads/report.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="22" count="22">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17" count="17">
   <x:si>
     <x:t>Name</x:t>
   </x:si>
@@ -22,64 +22,49 @@
     <x:t>E-mail</x:t>
   </x:si>
   <x:si>
+    <x:t>Employee_Code</x:t>
+  </x:si>
+  <x:si>
     <x:t>Policy_Id</x:t>
   </x:si>
   <x:si>
     <x:t>Policy_Status</x:t>
   </x:si>
   <x:si>
+    <x:t>Jayashree Kulai</x:t>
+  </x:si>
+  <x:si>
+    <x:t>jayashree.cs16@sahyadri.edu.in</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MNG001</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5fd0709530a434204c3007d5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Roy Pashan</x:t>
+  </x:si>
+  <x:si>
+    <x:t>mail2winstonroy@yahoo.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MNG002</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5fd0709530a434204c3007d5</x:t>
+  </x:si>
+  <x:si>
     <x:t>Winston Roy</x:t>
   </x:si>
   <x:si>
     <x:t>pashanwinsty1998@gmail.com</x:t>
   </x:si>
   <x:si>
-    <x:t>5fd320a7d28d01408a4c4e2a</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Vinayaka Naik</x:t>
-  </x:si>
-  <x:si>
-    <x:t>vinayakamudrai@gmail.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t>5fd320a7d28d01408a4c4e2a</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Jayashree Kulai</x:t>
-  </x:si>
-  <x:si>
-    <x:t>jayashree.cs16@sahyadri.edu.in</x:t>
-  </x:si>
-  <x:si>
-    <x:t>5fd320a7d28d01408a4c4e2a</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Sharal Linsha</x:t>
-  </x:si>
-  <x:si>
-    <x:t>sharalfonseca1810@gmail.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t>5fd320a7d28d01408a4c4e2a</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Vinusha Monterio</x:t>
-  </x:si>
-  <x:si>
-    <x:t>vinushamonteiro2016@gmail.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t>5fd320a7d28d01408a4c4e2a</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Roy pashan</x:t>
-  </x:si>
-  <x:si>
-    <x:t>mail2winstonroy@yahoo.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t>5fd320a7d28d01408a4c4e2a</x:t>
+    <x:t>AD002</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5fd0709530a434204c3007d5</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -442,7 +427,7 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="1" spans="1:4">
+    <x:row r="1" spans="1:5">
       <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -455,88 +440,58 @@
       <x:c r="D1" s="0" t="s">
         <x:v>3</x:v>
       </x:c>
+      <x:c r="E1" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
     </x:row>
-    <x:row r="2" spans="1:4">
+    <x:row r="2" spans="1:5">
       <x:c r="A2" s="0" t="s">
-        <x:v>4</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="C2" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="D2" s="0" t="b">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D2" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E2" s="0" t="b">
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="3" spans="1:4">
+    <x:row r="3" spans="1:5">
       <x:c r="A3" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="B3" s="0" t="s">
-        <x:v>8</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="C3" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="D3" s="0" t="b">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="D3" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="E3" s="0" t="b">
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="4" spans="1:4">
+    <x:row r="4" spans="1:5">
       <x:c r="A4" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="B4" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="C4" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="D4" s="0" t="b">
-        <x:v>0</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="5" spans="1:4">
-      <x:c r="A5" s="0" t="s">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="B5" s="0" t="s">
-        <x:v>14</x:v>
-      </x:c>
-      <x:c r="C5" s="0" t="s">
         <x:v>15</x:v>
       </x:c>
-      <x:c r="D5" s="0" t="b">
-        <x:v>0</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="6" spans="1:4">
-      <x:c r="A6" s="0" t="s">
+      <x:c r="D4" s="0" t="s">
         <x:v>16</x:v>
       </x:c>
-      <x:c r="B6" s="0" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="C6" s="0" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="D6" s="0" t="b">
-        <x:v>0</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="7" spans="1:4">
-      <x:c r="A7" s="0" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="B7" s="0" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="C7" s="0" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="D7" s="0" t="b">
+      <x:c r="E4" s="0" t="b">
         <x:v>0</x:v>
       </x:c>
     </x:row>

</xml_diff>